<commit_message>
[SAI - PQRS] configuración mensaje temporal por vacaciones. Se aplica a versión en campus en aurea y en aurea2.
</commit_message>
<xml_diff>
--- a/Documentación/Estructura_DB_30_SAI_solicitudes.xlsx
+++ b/Documentación/Estructura_DB_30_SAI_solicitudes.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Hoja3" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -167,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="513">
   <si>
     <t xml:space="preserve">App</t>
   </si>
@@ -1794,7 +1796,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1829,6 +1831,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB3A2C7"/>
         <bgColor rgb="FF9999FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -1884,7 +1892,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1974,6 +1982,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2163,10 +2175,10 @@
   </sheetPr>
   <dimension ref="A1:R409"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I77" activeCellId="0" sqref="I77"/>
+      <selection pane="bottomLeft" activeCell="C279" activeCellId="0" sqref="C279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4655,21 +4667,13 @@
       <c r="Q97" s="9"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1"/>
+    <row r="98" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="8" t="s">
         <v>176</v>
       </c>
       <c r="C98" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
-      <c r="I98" s="1"/>
-      <c r="J98" s="1"/>
       <c r="K98" s="1" t="n">
         <v>18</v>
       </c>
@@ -4695,8 +4699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1"/>
+    <row r="99" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="8" t="s">
         <v>177</v>
       </c>
@@ -4706,12 +4709,6 @@
       <c r="D99" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
-      <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
       <c r="K99" s="1" t="n">
         <v>19</v>
       </c>
@@ -4773,7 +4770,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1"/>
       <c r="B101" s="8" t="s">
         <v>186</v>
       </c>
@@ -4783,6 +4781,12 @@
       <c r="D101" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
       <c r="K101" s="1" t="n">
         <v>21</v>
       </c>
@@ -4808,19 +4812,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1"/>
       <c r="B102" s="13" t="s">
         <v>191</v>
       </c>
       <c r="C102" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
       <c r="K102" s="1" t="n">
         <v>22</v>
       </c>
       <c r="L102" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="M102" s="1"/>
       <c r="N102" s="9" t="s">
         <v>93</v>
       </c>
@@ -4831,6 +4844,7 @@
         <v>95</v>
       </c>
       <c r="Q102" s="9"/>
+      <c r="R102" s="1"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1"/>
@@ -8620,21 +8634,13 @@
       <c r="Q231" s="9"/>
       <c r="R231" s="1"/>
     </row>
-    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="1"/>
+    <row r="232" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B232" s="8" t="s">
         <v>331</v>
       </c>
       <c r="C232" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D232" s="1"/>
-      <c r="E232" s="1"/>
-      <c r="F232" s="1"/>
-      <c r="G232" s="1"/>
-      <c r="H232" s="1"/>
-      <c r="I232" s="1"/>
-      <c r="J232" s="1"/>
       <c r="K232" s="1" t="n">
         <v>22</v>
       </c>
@@ -8660,8 +8666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="1"/>
+    <row r="233" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B233" s="8" t="s">
         <v>332</v>
       </c>
@@ -8671,12 +8676,6 @@
       <c r="D233" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="E233" s="1"/>
-      <c r="F233" s="1"/>
-      <c r="G233" s="1"/>
-      <c r="H233" s="1"/>
-      <c r="I233" s="1"/>
-      <c r="J233" s="1"/>
       <c r="K233" s="1" t="n">
         <v>23</v>
       </c>
@@ -8738,7 +8737,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="235" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="1"/>
       <c r="B235" s="8" t="s">
         <v>334</v>
       </c>
@@ -8748,6 +8748,12 @@
       <c r="D235" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="E235" s="1"/>
+      <c r="F235" s="1"/>
+      <c r="G235" s="1"/>
+      <c r="H235" s="1"/>
+      <c r="I235" s="1"/>
+      <c r="J235" s="1"/>
       <c r="K235" s="1" t="n">
         <v>25</v>
       </c>
@@ -8773,19 +8779,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="236" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="1"/>
       <c r="B236" s="13" t="s">
         <v>335</v>
       </c>
       <c r="C236" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="D236" s="1"/>
+      <c r="E236" s="1"/>
+      <c r="F236" s="1"/>
+      <c r="G236" s="1"/>
+      <c r="H236" s="1"/>
+      <c r="I236" s="1"/>
+      <c r="J236" s="1"/>
       <c r="K236" s="1" t="n">
         <v>26</v>
       </c>
       <c r="L236" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="M236" s="1"/>
       <c r="N236" s="9" t="s">
         <v>93</v>
       </c>
@@ -8796,6 +8811,7 @@
         <v>95</v>
       </c>
       <c r="Q236" s="9"/>
+      <c r="R236" s="1"/>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1"/>
@@ -12636,4 +12652,1526 @@
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F78"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D71" activeCellId="0" sqref="D71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="1" width="22.51"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Campus - FAV] [SAI - FAV] [SAI - Registro Atenciones] Ajustes de integración de los canales de atención a una sola tabla.
</commit_message>
<xml_diff>
--- a/Documentación/Estructura_DB_30_SAI_solicitudes.xlsx
+++ b/Documentación/Estructura_DB_30_SAI_solicitudes.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Hoja2" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Hoja3" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Hoja4" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -168,8 +169,159 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Autoría desconocida</author>
+  </authors>
+  <commentList>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">MAURO: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Los tipos especiales son: 
+iTexto = 1
+iMoneda = 2
+iCombo = 3
+iMemo = 4
+iNumero = 5
+iConsecutivo = 6
+iFecha = 7
+iTercero = 8
+iBusqueda = 9
+iComboTexto = 13
+iBusquedaTexto = 19
+idEntidad = 51
+idTablaPadre = 52
+iAnexoDB = 91
+iAnexoId = 92</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Angel Mauro Avellaneda Barreto:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Tipos especiales:
+1 - Campo Oculto que se muestra
+2 - Campo Oculto que </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">NO se muestra
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">3 - Campo No Editable - Como si fuera llave
+31 - Combo Hijo.
+71 - Hora
+72 - Minuto
+73 - Hora Oculta
+74 - Minuto Oculto</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Mauro Avellaneda:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Tambien se usa para indicar si un bloque hijo es editable en cuadricula (valor de 3000 o superior)
+O si un bloque hijo se le cambia el orden, valores entre 2000 y 2999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Angel Mauro Avellaneda Barreto:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Si quiere un GrupoCampos despues del campo ponga -1
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="523">
   <si>
     <t xml:space="preserve">App</t>
   </si>
@@ -1708,6 +1860,36 @@
   </si>
   <si>
     <t xml:space="preserve">saiu73evalutilmotivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saiu73idcanal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saiu73idtelefono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saiu73numtelefono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saiu73numorigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saiu73idchat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saiu73numsesionchat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saiu73idcorreo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saiu73idcorreootro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saiu73correoorigen</t>
   </si>
 </sst>
 </file>
@@ -2175,13 +2357,13 @@
   </sheetPr>
   <dimension ref="A1:R409"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C279" activeCellId="0" sqref="C279"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A394" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="G346" activeCellId="0" sqref="G346"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.43"/>
   </cols>
@@ -12659,13 +12841,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D71" activeCellId="0" sqref="D71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="1" width="22.51"/>
@@ -12710,6 +12892,9 @@
       <c r="F2" s="1" t="s">
         <v>447</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -12730,6 +12915,9 @@
       <c r="F3" s="1" t="s">
         <v>450</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -12750,6 +12938,7 @@
       <c r="F4" s="1" t="s">
         <v>451</v>
       </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -12770,6 +12959,9 @@
       <c r="F5" s="1" t="s">
         <v>452</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -12790,6 +12982,9 @@
       <c r="F6" s="1" t="s">
         <v>453</v>
       </c>
+      <c r="G6" s="1" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -12852,6 +13047,9 @@
       <c r="F10" s="1" t="s">
         <v>457</v>
       </c>
+      <c r="G10" s="1" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -12872,6 +13070,9 @@
       <c r="F11" s="1" t="s">
         <v>458</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -12892,6 +13093,9 @@
       <c r="F12" s="1" t="s">
         <v>459</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -12912,6 +13116,9 @@
       <c r="F13" s="1" t="s">
         <v>460</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -12965,6 +13172,9 @@
       <c r="F17" s="1" t="s">
         <v>461</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -12985,6 +13195,9 @@
       <c r="F18" s="1" t="s">
         <v>462</v>
       </c>
+      <c r="G18" s="1" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -13005,6 +13218,9 @@
       <c r="F19" s="1" t="s">
         <v>463</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -13025,6 +13241,9 @@
       <c r="F20" s="1" t="s">
         <v>464</v>
       </c>
+      <c r="G20" s="1" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -13045,6 +13264,9 @@
       <c r="F21" s="1" t="s">
         <v>465</v>
       </c>
+      <c r="G21" s="1" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -13065,6 +13287,9 @@
       <c r="F22" s="1" t="s">
         <v>466</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -13085,6 +13310,9 @@
       <c r="F23" s="1" t="s">
         <v>467</v>
       </c>
+      <c r="G23" s="1" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -13105,6 +13333,9 @@
       <c r="F24" s="1" t="s">
         <v>468</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
@@ -13125,6 +13356,9 @@
       <c r="F25" s="1" t="s">
         <v>469</v>
       </c>
+      <c r="G25" s="1" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -13145,6 +13379,9 @@
       <c r="F26" s="1" t="s">
         <v>470</v>
       </c>
+      <c r="G26" s="1" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -13165,6 +13402,9 @@
       <c r="F27" s="1" t="s">
         <v>471</v>
       </c>
+      <c r="G27" s="1" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
@@ -13185,6 +13425,9 @@
       <c r="F28" s="1" t="s">
         <v>472</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -13205,6 +13448,9 @@
       <c r="F29" s="1" t="s">
         <v>473</v>
       </c>
+      <c r="G29" s="1" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
@@ -13239,6 +13485,9 @@
       <c r="F31" s="1" t="s">
         <v>474</v>
       </c>
+      <c r="G31" s="1" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -13259,6 +13508,9 @@
       <c r="F32" s="1" t="s">
         <v>475</v>
       </c>
+      <c r="G32" s="1" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -13279,6 +13531,9 @@
       <c r="F33" s="1" t="s">
         <v>476</v>
       </c>
+      <c r="G33" s="1" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -13299,6 +13554,9 @@
       <c r="F34" s="1" t="s">
         <v>477</v>
       </c>
+      <c r="G34" s="1" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -13319,6 +13577,9 @@
       <c r="F35" s="1" t="s">
         <v>478</v>
       </c>
+      <c r="G35" s="1" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
@@ -13339,6 +13600,9 @@
       <c r="F36" s="1" t="s">
         <v>479</v>
       </c>
+      <c r="G36" s="1" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
@@ -13359,6 +13623,9 @@
       <c r="F37" s="1" t="s">
         <v>480</v>
       </c>
+      <c r="G37" s="1" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
@@ -13379,6 +13646,7 @@
       <c r="F38" s="1" t="s">
         <v>481</v>
       </c>
+      <c r="G38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
@@ -13399,6 +13667,9 @@
       <c r="F39" s="1" t="s">
         <v>482</v>
       </c>
+      <c r="G39" s="1" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
@@ -13419,6 +13690,9 @@
       <c r="F40" s="1" t="s">
         <v>483</v>
       </c>
+      <c r="G40" s="1" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
@@ -13439,6 +13713,9 @@
       <c r="F41" s="1" t="s">
         <v>484</v>
       </c>
+      <c r="G41" s="1" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
@@ -13459,6 +13736,9 @@
       <c r="F42" s="1" t="s">
         <v>485</v>
       </c>
+      <c r="G42" s="1" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
@@ -13479,6 +13759,9 @@
       <c r="F43" s="1" t="s">
         <v>486</v>
       </c>
+      <c r="G43" s="1" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
@@ -13499,6 +13782,9 @@
       <c r="F44" s="1" t="s">
         <v>487</v>
       </c>
+      <c r="G44" s="1" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
@@ -13527,6 +13813,9 @@
       <c r="F46" s="1" t="s">
         <v>488</v>
       </c>
+      <c r="G46" s="1" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
@@ -13547,6 +13836,9 @@
       <c r="F47" s="1" t="s">
         <v>489</v>
       </c>
+      <c r="G47" s="1" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -13567,6 +13859,9 @@
       <c r="F48" s="1" t="s">
         <v>490</v>
       </c>
+      <c r="G48" s="1" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
@@ -13587,6 +13882,9 @@
       <c r="F49" s="1" t="s">
         <v>491</v>
       </c>
+      <c r="G49" s="1" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
@@ -13607,6 +13905,9 @@
       <c r="F50" s="1" t="s">
         <v>492</v>
       </c>
+      <c r="G50" s="1" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -13627,6 +13928,9 @@
       <c r="F51" s="1" t="s">
         <v>493</v>
       </c>
+      <c r="G51" s="1" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -13647,6 +13951,9 @@
       <c r="F52" s="1" t="s">
         <v>494</v>
       </c>
+      <c r="G52" s="1" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -13667,6 +13974,9 @@
       <c r="F53" s="1" t="s">
         <v>495</v>
       </c>
+      <c r="G53" s="1" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
@@ -13687,6 +13997,9 @@
       <c r="F54" s="1" t="s">
         <v>496</v>
       </c>
+      <c r="G54" s="1" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
@@ -13707,6 +14020,9 @@
       <c r="F55" s="1" t="s">
         <v>497</v>
       </c>
+      <c r="G55" s="1" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
@@ -13727,6 +14043,9 @@
       <c r="F56" s="1" t="s">
         <v>498</v>
       </c>
+      <c r="G56" s="1" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
@@ -13747,6 +14066,7 @@
       <c r="F57" s="1" t="s">
         <v>499</v>
       </c>
+      <c r="G57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
@@ -13767,6 +14087,7 @@
       <c r="F58" s="1" t="s">
         <v>500</v>
       </c>
+      <c r="G58" s="1"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -13787,6 +14108,7 @@
       <c r="F59" s="1" t="s">
         <v>501</v>
       </c>
+      <c r="G59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
@@ -13807,6 +14129,7 @@
       <c r="F60" s="1" t="s">
         <v>502</v>
       </c>
+      <c r="G60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
@@ -13827,6 +14150,7 @@
       <c r="F61" s="1" t="s">
         <v>503</v>
       </c>
+      <c r="G61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
@@ -13847,6 +14171,7 @@
       <c r="F62" s="1" t="s">
         <v>504</v>
       </c>
+      <c r="G62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
@@ -13867,6 +14192,7 @@
       <c r="F63" s="1" t="s">
         <v>505</v>
       </c>
+      <c r="G63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
@@ -13887,6 +14213,7 @@
       <c r="F64" s="1" t="s">
         <v>506</v>
       </c>
+      <c r="G64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
@@ -13907,6 +14234,7 @@
       <c r="F65" s="1" t="s">
         <v>507</v>
       </c>
+      <c r="G65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
@@ -13927,6 +14255,7 @@
       <c r="F66" s="1" t="s">
         <v>508</v>
       </c>
+      <c r="G66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
@@ -13947,6 +14276,7 @@
       <c r="F67" s="1" t="s">
         <v>509</v>
       </c>
+      <c r="G67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
@@ -13967,6 +14297,7 @@
       <c r="F68" s="1" t="s">
         <v>510</v>
       </c>
+      <c r="G68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
@@ -13987,6 +14318,7 @@
       <c r="F69" s="1" t="s">
         <v>511</v>
       </c>
+      <c r="G69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
@@ -14007,6 +14339,7 @@
       <c r="F70" s="1" t="s">
         <v>512</v>
       </c>
+      <c r="G70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
@@ -14069,99 +14402,99 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>50</v>
       </c>
     </row>
@@ -14174,4 +14507,1123 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:R65"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="L58" activeCellId="0" sqref="L58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>3073</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>3001</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="O15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="L18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="L19" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="L20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M20" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="R20" s="1" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L21" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="O21" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="L22" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M22" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="R22" s="1" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="L23" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M23" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="N23" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q23" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="R23" s="1" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="L25" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M25" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="N25" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="O25" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="R25" s="1" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="L26" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="M27" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="K28" s="1" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="L29" s="1" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="L30" s="1" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="L31" s="1" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="M32" s="1" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="L34" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="L35" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="M36" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="M37" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="M38" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="L39" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="M40" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="K41" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="L42" s="1" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="L43" s="1" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K44" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="M44" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="M45" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K46" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="M46" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="M47" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="M48" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="M49" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K50" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="M50" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="K51" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="M51" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K52" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="M52" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K53" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M53" s="1"/>
+      <c r="N53" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="O53" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="P53" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K54" s="1" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K55" s="1" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K56" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="L56" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N56" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="O56" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="P56" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K57" s="1" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K58" s="1" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="K59" s="1" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="K60" s="1" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K64" s="1"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K65" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>